<commit_message>
Upadting ClientSecurityHashKey Code (#96)
* Committed the first version of POC as a package

* Updated ClientSecurityHashKey Process

* updated ClientSecurityHashKey Process

Co-authored-by: Vajrang <vajrang@outlook.com>
</commit_message>
<xml_diff>
--- a/Manjushree/Week1_Calculator_RoboticEnterpriseFramework/Data/Input/input.xlsx
+++ b/Manjushree/Week1_Calculator_RoboticEnterpriseFramework/Data/Input/input.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\GitSpace\RPA-Developer-in-30-Days\vajrang\Week1Calculator_Reframework\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UiPath\RPA-Developer-in-30-Days\Manjushree\Week1_Calculator_RoboticEnterpriseFramework\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8872B9-BC25-43BC-97D1-BC1AE163CD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF65CB1A-9BB3-424B-A09F-B0EB90F3A539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>first</t>
   </si>
@@ -36,13 +36,49 @@
     <t>operand</t>
   </si>
   <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
     <t>+</t>
   </si>
   <si>
+    <t xml:space="preserve">8	
+</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10	
+</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
     <t>*</t>
   </si>
   <si>
+    <t xml:space="preserve">27	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5	
+</t>
+  </si>
+  <si>
     <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4	
+</t>
   </si>
 </sst>
 </file>
@@ -78,8 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,94 +400,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="B4" s="1">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="https://www.youtube.com/watch?v=4bTTO_ie58o&amp;list=PLFd2UxUMjZNfUqyCCB_zs0cI-7nEO4T8E" xr:uid="{812E8542-1EE5-40F4-A1C6-69F699F45AA0}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>